<commit_message>
patch 1.34 | fix pridanie vyroby aj na HH:30, pri kalendari sa zobrazuju cele hodiny ale vyroba sa zobrazuje po pol hodine
</commit_message>
<xml_diff>
--- a/public/vyrobky.xlsx
+++ b/public/vyrobky.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\Webiky\tpv-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C4751F-5029-4CD9-B502-F10BA29A64F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A97471C-16A4-4634-8253-6C21CE855D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diel" sheetId="1" r:id="rId1"/>
-    <sheet name="Hárok2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hárok3" sheetId="3" r:id="rId3"/>
+    <sheet name="bg unused" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>99-23-3426</t>
   </si>
@@ -48,117 +47,6 @@
     <t>cisloVykresu</t>
   </si>
   <si>
-    <t>7A1B034_0117</t>
-  </si>
-  <si>
-    <t>Plošina pre montáž PM50</t>
-  </si>
-  <si>
-    <t>Optima</t>
-  </si>
-  <si>
-    <t>65-34-7519</t>
-  </si>
-  <si>
-    <t>Senzorové telo ST100</t>
-  </si>
-  <si>
-    <t>MechaServis</t>
-  </si>
-  <si>
-    <t>9C2D048_0214</t>
-  </si>
-  <si>
-    <t>Závesný modul ZM35</t>
-  </si>
-  <si>
-    <t>Technoplast</t>
-  </si>
-  <si>
-    <t>33-12-8476</t>
-  </si>
-  <si>
-    <t>Puzdro prevodovky PP20</t>
-  </si>
-  <si>
-    <t>VibroTech</t>
-  </si>
-  <si>
-    <t>8E5F056_0318</t>
-  </si>
-  <si>
-    <t>Nástrojová hlava NH10</t>
-  </si>
-  <si>
-    <t>InnovaTools</t>
-  </si>
-  <si>
-    <t>47-23-6145</t>
-  </si>
-  <si>
-    <t>Rám stroja RS45</t>
-  </si>
-  <si>
-    <t>4G6H078_0415</t>
-  </si>
-  <si>
-    <t>Spojovacia tyč ST15</t>
-  </si>
-  <si>
-    <t>82-56-9457</t>
-  </si>
-  <si>
-    <t>TechnoParts</t>
-  </si>
-  <si>
-    <t>5J7K092_0519</t>
-  </si>
-  <si>
-    <t>Kryt ovládacieho modulu KM90</t>
-  </si>
-  <si>
-    <t>RotorTech</t>
-  </si>
-  <si>
-    <t>21-78-3641</t>
-  </si>
-  <si>
-    <t>Signalizačná jednotka SJ30</t>
-  </si>
-  <si>
-    <t>Microtron</t>
-  </si>
-  <si>
-    <t>3L8M104_0613</t>
-  </si>
-  <si>
-    <t>Nástavec pre frézu NF25</t>
-  </si>
-  <si>
-    <t>58-19-8352</t>
-  </si>
-  <si>
-    <t>Nosná konzola NK80</t>
-  </si>
-  <si>
-    <t>6N9P116_0717</t>
-  </si>
-  <si>
-    <t>Adaptér pre čerpadlo AC40</t>
-  </si>
-  <si>
-    <t>FlexiSystems</t>
-  </si>
-  <si>
-    <t>90-43-7268</t>
-  </si>
-  <si>
-    <t>Ložiskové teleso LT50</t>
-  </si>
-  <si>
-    <t>Mecano</t>
-  </si>
-  <si>
     <t>bg</t>
   </si>
   <si>
@@ -192,9 +80,6 @@
     <t>brownBG</t>
   </si>
   <si>
-    <t>Mechanický úzaver MU70</t>
-  </si>
-  <si>
     <t>lightBlueBG</t>
   </si>
   <si>
@@ -214,6 +99,60 @@
   </si>
   <si>
     <t>beigeBG</t>
+  </si>
+  <si>
+    <t>TaTech</t>
+  </si>
+  <si>
+    <t>Predny panel - CM IP</t>
+  </si>
+  <si>
+    <t>Zadny panel - CM IP</t>
+  </si>
+  <si>
+    <t>Lavy bocny panel - CM IP</t>
+  </si>
+  <si>
+    <t>Pravy bocny panel - CM IP</t>
+  </si>
+  <si>
+    <t>D_Plate</t>
+  </si>
+  <si>
+    <t>A_Teleso_V2</t>
+  </si>
+  <si>
+    <t>Stol</t>
+  </si>
+  <si>
+    <t>Skenerovy drziak KV30-cast Y</t>
+  </si>
+  <si>
+    <t>Trapez</t>
+  </si>
+  <si>
+    <t>54-24-3449</t>
+  </si>
+  <si>
+    <t>54-24-3450</t>
+  </si>
+  <si>
+    <t>54-24-3451</t>
+  </si>
+  <si>
+    <t>54-24-3459</t>
+  </si>
+  <si>
+    <t>0277-001</t>
+  </si>
+  <si>
+    <t>0277-002</t>
+  </si>
+  <si>
+    <t>99-23-3427</t>
+  </si>
+  <si>
+    <t>3-842-512-991</t>
   </si>
 </sst>
 </file>
@@ -273,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -286,6 +225,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -593,7 +538,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -621,7 +566,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -629,13 +574,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>46</v>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="2"/>
@@ -650,219 +595,174 @@
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>48</v>
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="E5"/>
       <c r="F5" s="3"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="A6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F6" s="3"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="6">
+        <v>30364882</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="5" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
       <c r="E13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
       <c r="E17"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -991,24 +891,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="31.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>